<commit_message>
Manejo de archivo de excel. Facturas enviadas a nueva hoja. Llamado a la Api con datos por defecto.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,17 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marif\Desktop\alegraApp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0E0606-975D-4DB2-AFB7-DEA08CE4EF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Pendientes" sheetId="1" r:id="rId1"/>
+    <sheet name="Facturados" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>FECHA</t>
   </si>
@@ -130,32 +151,39 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,11 +191,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -181,95 +215,106 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -459,20 +504,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,12 +591,12 @@
       </c>
       <c r="W1" s="8"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
-        <v>44366.0</v>
+        <v>44366</v>
       </c>
       <c r="B2" s="10">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>22</v>
@@ -569,7 +619,7 @@
         <v>27</v>
       </c>
       <c r="K2" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="16" t="s">
         <v>28</v>
@@ -584,30 +634,30 @@
         <v>31</v>
       </c>
       <c r="P2" s="18">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="Q2" s="19">
-        <v>1791.0</v>
+        <v>1791</v>
       </c>
       <c r="R2" s="19">
-        <f t="shared" ref="R2:R3" si="1">P2*Q2</f>
+        <f t="shared" ref="R2:R3" si="0">P2*Q2</f>
         <v>322380</v>
       </c>
       <c r="S2" s="19">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="T2" s="19">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="U2" s="19"/>
       <c r="V2" s="20"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
-        <v>44365.0</v>
+        <v>44365</v>
       </c>
       <c r="B3" s="10">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>32</v>
@@ -632,7 +682,7 @@
         <v>35</v>
       </c>
       <c r="K3" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="L3" s="16" t="s">
         <v>28</v>
@@ -645,18 +695,18 @@
         <v>37</v>
       </c>
       <c r="P3" s="18">
-        <v>204.0</v>
+        <v>204</v>
       </c>
       <c r="Q3" s="19">
         <f>IF(E3="",U3, ROUND(U3/(1+E3),0))</f>
         <v>1280</v>
       </c>
       <c r="R3" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>261120</v>
       </c>
       <c r="S3" s="19">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="T3" s="19"/>
       <c r="U3" s="19">
@@ -665,6 +715,90 @@
       <c r="V3" s="20"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D02F83-ADAB-4D98-96DD-BBFB0CFDC378}">
+  <dimension ref="A1:V1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Llamado a la Api. Borrado de facturas enviadas.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marif\Desktop\alegraApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0E0606-975D-4DB2-AFB7-DEA08CE4EF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667DAB37-B910-4F78-B219-5EF1950AB1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pendientes" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
   <si>
     <t>FECHA</t>
   </si>
@@ -106,9 +106,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>Arley Jose Varon Varon</t>
-  </si>
-  <si>
     <t>Armenia</t>
   </si>
   <si>
@@ -124,28 +121,22 @@
     <t>5 pacas</t>
   </si>
   <si>
-    <t>208</t>
-  </si>
-  <si>
     <t>Fibra pp 12000 200 gr surtida</t>
   </si>
   <si>
     <t>Facturado</t>
   </si>
   <si>
-    <t>Estella González Arias</t>
-  </si>
-  <si>
     <t>Tuluá</t>
   </si>
   <si>
     <t>015751</t>
   </si>
   <si>
-    <t>957</t>
-  </si>
-  <si>
     <t>Soga cabuya 1/2 13mm 204m</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -516,8 +507,8 @@
   </sheetPr>
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -605,33 +596,33 @@
         <v>23</v>
       </c>
       <c r="E2" s="11"/>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="12">
+        <v>1</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>25</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>26</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>27</v>
       </c>
       <c r="K2" s="16">
         <v>1</v>
       </c>
       <c r="L2" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="N2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="16" t="s">
         <v>29</v>
-      </c>
-      <c r="N2" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>31</v>
       </c>
       <c r="P2" s="18">
         <v>180</v>
@@ -660,7 +651,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>23</v>
@@ -668,31 +659,31 @@
       <c r="E3" s="21">
         <v>0.19</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>33</v>
+      <c r="F3" s="12">
+        <v>1</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H3" s="13"/>
       <c r="I3" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K3" s="16">
         <v>1</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M3" s="10"/>
       <c r="N3" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="P3" s="18">
         <v>204</v>
@@ -723,7 +714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D02F83-ADAB-4D98-96DD-BBFB0CFDC378}">
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>

</xml_diff>